<commit_message>
validate preview and add unit id
</commit_message>
<xml_diff>
--- a/Resource/TestExcel/TestEcelMaterials.xlsx
+++ b/Resource/TestExcel/TestEcelMaterials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vtnghia\Documents\GitHub\CukCuk-G-2\Resource\TestExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\MISA-CukCuk-Duplicate\Resource\TestExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFEF766-35B2-430A-9EC4-385CA0CF7C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AC75F6-C39F-4D28-BAEF-86EC9B4FF454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="1140" windowWidth="21600" windowHeight="11385" xr2:uid="{13D47D62-CEEE-495D-9652-C4862B71A8E0}"/>
+    <workbookView xWindow="1830" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{13D47D62-CEEE-495D-9652-C4862B71A8E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Mã Nguyên vật liệu</t>
   </si>
@@ -58,9 +58,6 @@
     <t>BH-60817</t>
   </si>
   <si>
-    <t>Bia tươi</t>
-  </si>
-  <si>
     <t>Nhập khẩu</t>
   </si>
   <si>
@@ -74,6 +71,39 @@
   </si>
   <si>
     <t>Hello world</t>
+  </si>
+  <si>
+    <t>Xe hơi</t>
+  </si>
+  <si>
+    <t>Nhóm 3</t>
+  </si>
+  <si>
+    <t>Nhóm 4</t>
+  </si>
+  <si>
+    <t>Nhóm 5</t>
+  </si>
+  <si>
+    <t>Bia tươi1</t>
+  </si>
+  <si>
+    <t>Bia tươi2</t>
+  </si>
+  <si>
+    <t>Bia tươi3</t>
+  </si>
+  <si>
+    <t>Bia tươi4</t>
+  </si>
+  <si>
+    <t>BH-60819</t>
+  </si>
+  <si>
+    <t>BH-60818</t>
+  </si>
+  <si>
+    <t>BH-60820</t>
   </si>
 </sst>
 </file>
@@ -442,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C469519B-4182-4D78-B939-7576C518807F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,30 +514,86 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>